<commit_message>
Categorizacao Clientes - alterada
</commit_message>
<xml_diff>
--- a/rfm_categorizacao_padrao.xlsx
+++ b/rfm_categorizacao_padrao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f6f29faf5b640946/Área de Trabalho/UpData/rfm_ecommerce/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{AEA875C2-C5BA-42AC-899E-ECB15F325DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8266B00B-7499-4CE8-AB3C-DA18AE1766DA}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{AEA875C2-C5BA-42AC-899E-ECB15F325DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A259F966-EF1E-4A17-973A-ABB91011BC24}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BD0EB3F7-1B60-4492-A5C7-D183E8E3BF54}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Recem Ativos</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -152,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -162,9 +165,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -173,8 +173,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,13 +523,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+      <c r="A2" s="16"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="16"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -542,7 +544,7 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +562,7 @@
       <c r="C1" s="5">
         <v>1</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>0</v>
       </c>
     </row>
@@ -574,7 +576,7 @@
       <c r="C2" s="5">
         <v>2</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -588,7 +590,7 @@
       <c r="C3" s="5">
         <v>3</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>2</v>
       </c>
     </row>
@@ -602,7 +604,7 @@
       <c r="C4" s="5">
         <v>4</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="G4" t="s">
@@ -619,7 +621,7 @@
       <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -644,7 +646,7 @@
       <c r="C7" s="5">
         <v>3</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -669,7 +671,7 @@
       <c r="C9" s="6">
         <v>1</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>6</v>
       </c>
     </row>
@@ -751,46 +753,46 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
-        <v>2</v>
-      </c>
-      <c r="B17" s="16">
-        <v>1</v>
-      </c>
-      <c r="C17" s="16">
+      <c r="A17" s="15">
+        <v>2</v>
+      </c>
+      <c r="B17" s="15">
+        <v>1</v>
+      </c>
+      <c r="C17" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
-        <v>2</v>
-      </c>
-      <c r="B18" s="16">
-        <v>1</v>
-      </c>
-      <c r="C18" s="16">
+      <c r="A18" s="15">
+        <v>2</v>
+      </c>
+      <c r="B18" s="15">
+        <v>1</v>
+      </c>
+      <c r="C18" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
-        <v>2</v>
-      </c>
-      <c r="B19" s="17">
-        <v>1</v>
-      </c>
-      <c r="C19" s="17">
+      <c r="A19" s="2">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
-        <v>2</v>
-      </c>
-      <c r="B20" s="13">
-        <v>1</v>
-      </c>
-      <c r="C20" s="13">
+      <c r="A20" s="12">
+        <v>2</v>
+      </c>
+      <c r="B20" s="12">
+        <v>1</v>
+      </c>
+      <c r="C20" s="12">
         <v>4</v>
       </c>
     </row>
@@ -827,7 +829,7 @@
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -841,7 +843,7 @@
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>